<commit_message>
Adatbázis bővült a hicp-vel (ez MoM-ben volt, QoQ-ba konvertáltam).
Kész vannak az előrejelzések a GDP-re nem gördülő mintán.
</commit_message>
<xml_diff>
--- a/data/ger_gdp_hicp.xlsx
+++ b/data/ger_gdp_hicp.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Munka1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
@@ -395,7 +392,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -551,6 +548,8 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="33">
@@ -901,7 +900,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="1. jelölőszín" xfId="18" builtinId="29" customBuiltin="1"/>
@@ -959,19 +958,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Orders"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1546,7 +1532,7 @@
         <v>106.1951</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1563,7 +1549,7 @@
         <v>104.21810000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1580,7 +1566,7 @@
         <v>104.05070000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1597,7 +1583,7 @@
         <v>102.35039999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1614,7 +1600,7 @@
         <v>103.18389999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1631,7 +1617,7 @@
         <v>103.71729999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1648,7 +1634,7 @@
         <v>104.7175</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1665,7 +1651,7 @@
         <v>105.1842</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1682,7 +1668,7 @@
         <v>104.6174</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1699,7 +1685,7 @@
         <v>104.084</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1715,8 +1701,11 @@
       <c r="E26">
         <v>103.8173</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>81.402003333333326</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1732,8 +1721,11 @@
       <c r="E27">
         <v>103.98399999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>81.688130000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1749,8 +1741,11 @@
       <c r="E28">
         <v>104.184</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>81.902716666666677</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1766,8 +1761,11 @@
       <c r="E29">
         <v>102.7505</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>81.866953333333342</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1783,8 +1781,11 @@
       <c r="E30">
         <v>102.4837</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>82.689556666666661</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -1800,8 +1801,11 @@
       <c r="E31">
         <v>103.15049999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>82.796853333333331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1817,8 +1821,11 @@
       <c r="E32">
         <v>100.8168</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>83.226036666666673</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -1834,8 +1841,11 @@
       <c r="E33">
         <v>101.51690000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>83.082973333333328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1851,8 +1861,11 @@
       <c r="E34">
         <v>102.8505</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>83.190269999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1868,8 +1881,11 @@
       <c r="E35">
         <v>101.4169</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>83.512159999999994</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1885,8 +1901,11 @@
       <c r="E36">
         <v>102.2504</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>83.72675333333332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1902,8 +1921,11 @@
       <c r="E37">
         <v>103.2505</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>83.369100000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1919,8 +1941,11 @@
       <c r="E38">
         <v>103.2839</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>83.44062666666666</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1936,8 +1961,11 @@
       <c r="E39">
         <v>101.2835</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>83.941346666666661</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1953,8 +1981,11 @@
       <c r="E40">
         <v>101.0502</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>84.334763333333328</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1970,8 +2001,11 @@
       <c r="E41">
         <v>102.4837</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>84.227466666666672</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -1987,8 +2021,11 @@
       <c r="E42">
         <v>103.0838</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>84.72818333333332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2004,8 +2041,11 @@
       <c r="E43">
         <v>103.71729999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>84.835480000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2021,8 +2061,11 @@
       <c r="E44">
         <v>102.61709999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>85.336189999999988</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -2038,8 +2081,11 @@
       <c r="E45">
         <v>103.1172</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>85.658083333333323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -2055,8 +2101,11 @@
       <c r="E46">
         <v>104.184</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>86.08726999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -2072,8 +2121,11 @@
       <c r="E47">
         <v>103.71729999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>86.909873333333323</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -2089,8 +2141,11 @@
       <c r="E48">
         <v>103.0505</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>87.160233333333323</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -2106,8 +2161,11 @@
       <c r="E49">
         <v>102.4837</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>86.874106666666663</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>44</v>
       </c>
@@ -2123,8 +2181,11 @@
       <c r="E50">
         <v>100.05</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>87.804003333333341</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -2140,8 +2201,11 @@
       <c r="E51">
         <v>100.98350000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>87.911296666666658</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -2157,8 +2221,11 @@
       <c r="E52">
         <v>101.1835</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>88.090130000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -2174,8 +2241,11 @@
       <c r="E53">
         <v>100.68340000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>87.982829999999993</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -2191,8 +2261,11 @@
       <c r="E54">
         <v>99.283209999999997</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>88.805436666666665</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -2208,8 +2281,11 @@
       <c r="E55">
         <v>99.883319999999998</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>88.66237000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>50</v>
       </c>
@@ -2225,8 +2301,11 @@
       <c r="E56">
         <v>99.549930000000003</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>89.020026666666652</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -2242,8 +2321,11 @@
       <c r="E57">
         <v>100.11669999999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>88.984263333333331</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -2259,8 +2341,11 @@
       <c r="E58">
         <v>100.9502</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>89.735336666666669</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -2276,8 +2361,11 @@
       <c r="E59">
         <v>101.25020000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>90.379116666666661</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>54</v>
       </c>
@@ -2293,8 +2381,11 @@
       <c r="E60">
         <v>101.2169</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>90.772530000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -2310,8 +2401,11 @@
       <c r="E61">
         <v>101.6836</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>90.879830000000013</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>56</v>
       </c>
@@ -2327,8 +2421,11 @@
       <c r="E62">
         <v>103.0172</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>91.27324666666668</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>57</v>
       </c>
@@ -2344,8 +2441,11 @@
       <c r="E63">
         <v>102.217</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>91.881259999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>58</v>
       </c>
@@ -2361,8 +2461,11 @@
       <c r="E64">
         <v>102.7838</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>92.668099999999995</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>59</v>
       </c>
@@ -2378,8 +2481,11 @@
       <c r="E65">
         <v>102.7838</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>92.989983333333328</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>60</v>
       </c>
@@ -2395,8 +2501,11 @@
       <c r="E66">
         <v>102.7171</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>93.168813333333333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>61</v>
       </c>
@@ -2412,8 +2521,11 @@
       <c r="E67">
         <v>103.3506</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>93.848356666666675</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>62</v>
       </c>
@@ -2429,8 +2541,11 @@
       <c r="E68">
         <v>102.5504</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>94.206006666666667</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>63</v>
       </c>
@@ -2446,8 +2561,11 @@
       <c r="E69">
         <v>103.48390000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>94.206009999999992</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -2463,8 +2581,11 @@
       <c r="E70">
         <v>102.1504</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <v>94.885553333333334</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>65</v>
       </c>
@@ -2480,8 +2601,11 @@
       <c r="E71">
         <v>102.5171</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <v>95.708153333333328</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>66</v>
       </c>
@@ -2497,8 +2621,11 @@
       <c r="E72">
         <v>101.917</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <v>96.280399999999986</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>67</v>
       </c>
@@ -2514,8 +2641,11 @@
       <c r="E73">
         <v>100.5168</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <v>97.031473333333338</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>68</v>
       </c>
@@ -2531,8 +2661,11 @@
       <c r="E74">
         <v>101.9837</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>97.818313333333322</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>69</v>
       </c>
@@ -2548,8 +2681,11 @@
       <c r="E75">
         <v>100.7835</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>98.605149999999995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -2565,8 +2701,11 @@
       <c r="E76">
         <v>101.5836</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>99.391983333333329</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>71</v>
       </c>
@@ -2582,8 +2721,11 @@
       <c r="E77">
         <v>102.05029999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>98.676683333333344</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>72</v>
       </c>
@@ -2599,8 +2741,11 @@
       <c r="E78">
         <v>98.983159999999998</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <v>98.569383333333334</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>73</v>
       </c>
@@ -2616,8 +2761,11 @@
       <c r="E79">
         <v>98.516419999999997</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <v>98.783976666666661</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>74</v>
       </c>
@@ -2633,8 +2781,11 @@
       <c r="E80">
         <v>98.283050000000003</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>98.998566666666662</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>75</v>
       </c>
@@ -2650,8 +2801,11 @@
       <c r="E81">
         <v>99.416569999999993</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>99.070100000000011</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>76</v>
       </c>
@@ -2667,8 +2821,11 @@
       <c r="E82">
         <v>99.016499999999994</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>99.391986666666654</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>77</v>
       </c>
@@ -2684,8 +2841,11 @@
       <c r="E83">
         <v>100.15</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>99.821169999999995</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>78</v>
       </c>
@@ -2701,8 +2861,11 @@
       <c r="E84">
         <v>100.8835</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>100.14306666666666</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -2718,8 +2881,11 @@
       <c r="E85">
         <v>100.38339999999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>100.60803333333335</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -2735,8 +2901,11 @@
       <c r="E86">
         <v>100.98350000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>101.50213333333333</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>81</v>
       </c>
@@ -2752,8 +2921,11 @@
       <c r="E87">
         <v>100.3501</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>102.32473333333333</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>82</v>
       </c>
@@ -2769,8 +2941,11 @@
       <c r="E88">
         <v>101.55029999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>102.82546666666667</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>83</v>
       </c>
@@ -2786,8 +2961,11 @@
       <c r="E89">
         <v>101.6169</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>103.25466666666667</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>84</v>
       </c>
@@ -2803,8 +2981,11 @@
       <c r="E90">
         <v>100.71680000000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>103.93419999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -2820,8 +3001,11 @@
       <c r="E91">
         <v>101.4169</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>104.47063333333334</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>86</v>
       </c>
@@ -2837,8 +3021,11 @@
       <c r="E92">
         <v>101.1169</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>104.93560000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>87</v>
       </c>
@@ -2854,8 +3041,11 @@
       <c r="E93">
         <v>100.4834</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>105.25749999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>88</v>
       </c>
@@ -2871,8 +3061,11 @@
       <c r="E94">
         <v>101.0835</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>105.82976666666667</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>89</v>
       </c>
@@ -2888,8 +3081,11 @@
       <c r="E95">
         <v>101.3502</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>106.04436666666668</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>90</v>
       </c>
@@ -2905,8 +3101,11 @@
       <c r="E96">
         <v>101.6169</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>106.68816666666667</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>91</v>
       </c>
@@ -2922,8 +3121,11 @@
       <c r="E97">
         <v>101.2835</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>106.7239</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>92</v>
       </c>
@@ -2939,8 +3141,11 @@
       <c r="E98">
         <v>102.5504</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>106.86696666666667</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>93</v>
       </c>
@@ -2956,8 +3161,11 @@
       <c r="E99">
         <v>102.5171</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>107.04576666666668</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>94</v>
       </c>
@@ -2973,8 +3181,11 @@
       <c r="E100">
         <v>102.3171</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>107.5107</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>95</v>
       </c>
@@ -2990,8 +3201,11 @@
       <c r="E101">
         <v>103.5506</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <v>107.1888</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>96</v>
       </c>
@@ -3007,8 +3221,11 @@
       <c r="E102">
         <v>104.85080000000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <v>106.79543333333334</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>97</v>
       </c>
@@ -3024,8 +3241,11 @@
       <c r="E103">
         <v>104.9508</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103">
+        <v>107.43916666666667</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>98</v>
       </c>
@@ -3041,8 +3261,11 @@
       <c r="E104">
         <v>105.6176</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104">
+        <v>107.54646666666667</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>99</v>
       </c>
@@ -3058,8 +3281,11 @@
       <c r="E105">
         <v>105.8176</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105">
+        <v>107.40339999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>100</v>
       </c>
@@ -3075,8 +3301,11 @@
       <c r="E106">
         <v>106.51779999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106">
+        <v>106.90273333333333</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>101</v>
       </c>
@@ -3092,8 +3321,11 @@
       <c r="E107">
         <v>106.3511</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107">
+        <v>107.40339999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>102</v>
       </c>
@@ -3109,8 +3341,11 @@
       <c r="E108">
         <v>106.6511</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108">
+        <v>107.97566666666667</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>103</v>
       </c>
@@ -3126,13 +3361,19 @@
       <c r="E109">
         <v>107.4179</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109">
+        <v>108.51216666666666</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>110</v>
       </c>
       <c r="D110">
         <v>113.0252</v>
+      </c>
+      <c r="F110">
+        <v>108.90560000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3148,6 +3389,7 @@
     <hyperlink ref="L1" r:id="rId9"/>
     <hyperlink ref="H1" r:id="rId10"/>
     <hyperlink ref="I1" r:id="rId11"/>
+    <hyperlink ref="F1" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>